<commit_message>
Use unscaled data and derive more columns
</commit_message>
<xml_diff>
--- a/public/web_model/template.xlsx
+++ b/public/web_model/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\stage\CRISP\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\stage\CRISP\public\web_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA3FDDB8-6CCC-4575-A451-78C6E5B7272F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF93D41-119C-4E18-8B59-3BCE9CE576B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{28EB074A-B6E7-4FF4-9E0E-6C4DA293FACA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>PATNR</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>Sex</t>
-  </si>
-  <si>
-    <t>Age_Early</t>
-  </si>
-  <si>
-    <t>Age_Late</t>
   </si>
   <si>
     <t>Pijn_acromioclaviaculair R</t>
@@ -797,15 +791,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1770448-8847-4091-BEBE-01B00610DEBD}">
-  <dimension ref="A1:DZ1"/>
+  <dimension ref="A1:DX1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BF17" sqref="BF17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:DY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1189,12 +1183,6 @@
       </c>
       <c r="DX1" t="s">
         <v>127</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>128</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>